<commit_message>
build file upload test
</commit_message>
<xml_diff>
--- a/src/assets/scholarship_approval.xlsx
+++ b/src/assets/scholarship_approval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sungjinpark/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D4E8DB9-96D2-634F-B1AE-3A3469B71AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C489872E-947E-EF4C-93FD-5E5413609767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="2720" windowWidth="28300" windowHeight="17440" xr2:uid="{3FE9D6A6-297E-0847-A38B-08AD90047BDE}"/>
+    <workbookView xWindow="38600" yWindow="8440" windowWidth="30240" windowHeight="18880" xr2:uid="{3FE9D6A6-297E-0847-A38B-08AD90047BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,25 +36,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>학번</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>학기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가중치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학생명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학생 학기수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 가중치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22200000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김한동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100만원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -101,8 +121,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -419,29 +442,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C365441E-59F5-C04F-8E77-09B67609EF76}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hotfix: 중복 콜 수정 (#54)
* feat: MUI 테이블 추가

* feat: MUI 테이블 추가

* feat: Student router 설정

* chore: fixed page name

* chore: fixed page name

* chore: 이름처리

* feat: 학생 CRUD

* chore: fixed modal layout

* feat: 학생 관리 페이지 API 연동

* feat[#2] 마일리지 장학금 신청 페이지

* feat[#2] 마일리지 장학금 신청자 관리 페이지

* fix[#2] 마일리지 장학금 신청자 관리 페이지 수정

* feat[#24] 관리자 권한 페이지 완성

* feat[#24] 마일리지 신청자 페이지 틀 구현

* hotfix: admin management name fix

* hotfix: deleted 중복 import

* feat[#27] 장학금 수혜 페이지 구현

* feat[#27] scholarship API 연동

* feat[#27] scholarship 페이지 탭

* feat[#27] 장학금 페이지 분리

* [feat#34] 카테고리, 학부, 전공 관리 페이지 구현

* fix[#34] API 연동 문제 해결

* feat[#34] 학부, 전공, 카테고리 필드 추가

* [fix#34] 장학금 신청자 페이지 수정

* fix: 장학금 수혜자 페이지

* fix[#34] Scholarship API 하드코딩 수정

* build file upload test

* hotfix: 중복 call 수정
</commit_message>
<xml_diff>
--- a/src/assets/scholarship_approval.xlsx
+++ b/src/assets/scholarship_approval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sungjinpark/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D4E8DB9-96D2-634F-B1AE-3A3469B71AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C489872E-947E-EF4C-93FD-5E5413609767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="2720" windowWidth="28300" windowHeight="17440" xr2:uid="{3FE9D6A6-297E-0847-A38B-08AD90047BDE}"/>
+    <workbookView xWindow="38600" yWindow="8440" windowWidth="30240" windowHeight="18880" xr2:uid="{3FE9D6A6-297E-0847-A38B-08AD90047BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,25 +36,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>학번</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>학기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가중치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학생명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학생 학기수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 가중치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22200000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김한동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100만원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -101,8 +121,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -419,29 +442,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C365441E-59F5-C04F-8E77-09B67609EF76}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>